<commit_message>
sune da up file indexing 2 problem 645
</commit_message>
<xml_diff>
--- a/Phan_cong_nhiem_vu.xlsx
+++ b/Phan_cong_nhiem_vu.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>Group</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Complete2</t>
+  </si>
+  <si>
+    <t>Complete3</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>IndexingI</t>
+  </si>
+  <si>
+    <t>MatrixPatternI</t>
+  </si>
+  <si>
+    <t>Minh</t>
+  </si>
+  <si>
+    <t>Complete1</t>
+  </si>
+  <si>
+    <t>Tu</t>
+  </si>
+  <si>
+    <t>Complete2</t>
+  </si>
+  <si>
+    <t>Nhat</t>
   </si>
   <si>
     <t>Complete3</t>
@@ -557,30 +584,30 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.3">
       <c r="A1" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.3">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0">
         <v>856</v>
@@ -603,7 +630,7 @@
     </row>
     <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0">
         <v>924</v>
@@ -626,7 +653,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0">
         <v>867</v>
@@ -649,7 +676,7 @@
     </row>
     <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0">
         <v>824</v>
@@ -672,7 +699,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0">
         <v>640</v>
@@ -695,7 +722,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0">
         <v>576</v>
@@ -718,7 +745,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0">
         <v>367</v>
@@ -741,7 +768,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B9" s="0">
         <v>885</v>
@@ -764,7 +791,7 @@
     </row>
     <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B10" s="0">
         <v>1463</v>
@@ -787,7 +814,7 @@
     </row>
     <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0">
         <v>1325</v>
@@ -810,7 +837,7 @@
     </row>
     <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0">
         <v>985</v>
@@ -833,7 +860,7 @@
     </row>
     <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0">
         <v>742</v>
@@ -856,7 +883,7 @@
     </row>
     <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0">
         <v>514</v>

</xml_diff>